<commit_message>
modif algorithme creation des nouvelles tables
</commit_message>
<xml_diff>
--- a/storage/app/public/observations_anatypes.xlsx
+++ b/storage/app/public/observations_anatypes.xlsx
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,16 +1015,16 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1041,10 +1041,10 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1061,10 +1061,10 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1081,10 +1081,10 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1101,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1118,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1135,10 +1135,10 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1152,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1177,7 +1177,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1191,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1205,7 +1205,7 @@
         <v>2</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1222,10 +1222,10 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1242,10 +1242,10 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1262,10 +1262,10 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1282,10 +1282,10 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1316,10 +1316,10 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1336,10 +1336,10 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1370,10 +1370,10 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1404,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1432,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1446,7 +1446,7 @@
         <v>3</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1460,7 +1460,7 @@
         <v>3</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1474,7 +1474,7 @@
         <v>3</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -1488,7 +1488,7 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1558,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Modification des observations et anatype
</commit_message>
<xml_diff>
--- a/storage/app/public/observations_anatypes.xlsx
+++ b/storage/app/public/observations_anatypes.xlsx
@@ -13,13 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="lab_observations-1" sheetId="1" r:id="rId1"/>
+    <sheet name="lab_observations-1 (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="especes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="51">
   <si>
     <t>id</t>
   </si>
@@ -27,9 +29,6 @@
     <t>intitule</t>
   </si>
   <si>
-    <t>categorie_id</t>
-  </si>
-  <si>
     <t>J`ai des animaux qui maigrissent</t>
   </si>
   <si>
@@ -154,6 +153,27 @@
   </si>
   <si>
     <t>RESIST</t>
+  </si>
+  <si>
+    <t>ANATYPE</t>
+  </si>
+  <si>
+    <t>OBSERVATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          [ 'anaacte_id' =&gt; 1, 'observation_id' =&gt; 1,],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['anatype_id' =&gt; </t>
+  </si>
+  <si>
+    <t>,],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, 'observation_id' =&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, 'espece_id' =&gt; </t>
   </si>
 </sst>
 </file>
@@ -960,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,7 +992,7 @@
     <col min="2" max="2" width="65.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -980,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>39</v>
@@ -997,610 +1017,2294 @@
       <c r="H1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
       <c r="F2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="F3">
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="F5">
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8">
-        <v>1</v>
+      <c r="F8">
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="E9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="H11">
+        <v>11</v>
+      </c>
+      <c r="G11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="G12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="I13">
+        <v>13</v>
+      </c>
+      <c r="H13">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="H14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>4</v>
-      </c>
-      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="H15">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="G16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
         <v>2</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
         <v>2</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>2</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
         <v>2</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="E26">
+        <v>26</v>
+      </c>
+      <c r="D26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="H27">
+        <v>27</v>
+      </c>
+      <c r="G27">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="G28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="G29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30">
-        <v>3</v>
-      </c>
-      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="D30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.44140625" customWidth="1"/>
+    <col min="9" max="9" width="37.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE(A2,B2,C2,D2,E2)</f>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 1,],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F66" si="0">CONCATENATE(A3,B3,C3,D3,E3)</f>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 2,],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 3,],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 4,],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 5,],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 6,],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 7,],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 13,],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 14,],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 15,],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 16,],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 17,],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 18,],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 19,],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 20,],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 21,],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 22,],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 23,],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 24,],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 30,],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 31,],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23">
+        <v>32</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 32,],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 34,],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 35,],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 36,],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'observation_id' =&gt; 37,],</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'observation_id' =&gt; 1,],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'observation_id' =&gt; 15,],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'observation_id' =&gt; 16,],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'observation_id' =&gt; 18,],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'observation_id' =&gt; 19,],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33">
+        <v>21</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'observation_id' =&gt; 21,],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34">
+        <v>25</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'observation_id' =&gt; 25,],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35">
+        <v>29</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'observation_id' =&gt; 29,],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 3, 'observation_id' =&gt; 1,],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 3, 'observation_id' =&gt; 8,],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
       <c r="D38">
         <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 1,],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 2,],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 3,],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 4,],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 5,],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 6,],</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 7,],</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45">
+        <v>13</v>
+      </c>
+      <c r="E45" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 13,],</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 14,],</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47">
+        <v>15</v>
+      </c>
+      <c r="E47" t="s">
+        <v>48</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 15,],</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48">
+        <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 16,],</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 18,],</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 19,],</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51">
+        <v>21</v>
+      </c>
+      <c r="E51" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 21,],</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52">
+        <v>23</v>
+      </c>
+      <c r="E52" t="s">
+        <v>48</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 23,],</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53">
+        <v>27</v>
+      </c>
+      <c r="E53" t="s">
+        <v>48</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 27,],</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54">
+        <v>28</v>
+      </c>
+      <c r="E54" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 28,],</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55">
+        <v>34</v>
+      </c>
+      <c r="E55" t="s">
+        <v>48</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'observation_id' =&gt; 34,],</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>48</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'observation_id' =&gt; 1,],</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'observation_id' =&gt; 2,],</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'observation_id' =&gt; 3,],</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>48</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'observation_id' =&gt; 4,],</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60">
+        <v>7</v>
+      </c>
+      <c r="E60" t="s">
+        <v>48</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'observation_id' =&gt; 7,],</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61">
+        <v>10</v>
+      </c>
+      <c r="E61" t="s">
+        <v>48</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'observation_id' =&gt; 10,],</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s">
+        <v>49</v>
+      </c>
+      <c r="D62">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>48</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'observation_id' =&gt; 11,],</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63">
+        <v>26</v>
+      </c>
+      <c r="E63" t="s">
+        <v>48</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'observation_id' =&gt; 26,],</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>49</v>
+      </c>
+      <c r="D64">
+        <v>12</v>
+      </c>
+      <c r="E64" t="s">
+        <v>48</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 6, 'observation_id' =&gt; 12,],</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65">
+        <v>13</v>
+      </c>
+      <c r="E65" t="s">
+        <v>48</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 6, 'observation_id' =&gt; 13,],</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66" t="s">
+        <v>49</v>
+      </c>
+      <c r="D66">
+        <v>14</v>
+      </c>
+      <c r="E66" t="s">
+        <v>48</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 6, 'observation_id' =&gt; 14,],</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B2:C223">
+    <sortCondition ref="B2:B223"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="39" customWidth="1"/>
+    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE(A2,B2,C2,D2,E2)</f>
+        <v>['anatype_id' =&gt; 1, 'espece_id' =&gt; 2,],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F19" si="0">CONCATENATE(A3,B3,C3,D3,E3)</f>
+        <v>['anatype_id' =&gt; 1, 'espece_id' =&gt; 3,],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'espece_id' =&gt; 6,],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'espece_id' =&gt; 7,],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 1, 'espece_id' =&gt; 8,],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'espece_id' =&gt; 2,],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 2, 'espece_id' =&gt; 3,],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 3, 'espece_id' =&gt; 2,],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 3, 'espece_id' =&gt; 3,],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'espece_id' =&gt; 2,],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 4, 'espece_id' =&gt; 3,],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'espece_id' =&gt; 2,],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 5, 'espece_id' =&gt; 3,],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 6, 'espece_id' =&gt; 2,],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 6, 'espece_id' =&gt; 3,],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 6, 'espece_id' =&gt; 6,],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 6, 'espece_id' =&gt; 7,],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>['anatype_id' =&gt; 6, 'espece_id' =&gt; 8,],</v>
       </c>
     </row>
   </sheetData>

</xml_diff>